<commit_message>
Added support for merge import
</commit_message>
<xml_diff>
--- a/tests/test_import/data_files_for_import_tests/data_file_study_labels_errors_merge.xlsx
+++ b/tests/test_import/data_files_for_import_tests/data_file_study_labels_errors_merge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="55">
   <si>
     <t>patient</t>
   </si>
@@ -166,16 +166,19 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>famhhist_cardiomyopat</t>
-  </si>
-  <si>
-    <t>famhisthalopathy</t>
-  </si>
-  <si>
-    <t>famhist_dimell</t>
-  </si>
-  <si>
-    <t>famhist_d</t>
+    <t>famhist_deaf</t>
+  </si>
+  <si>
+    <t>famhist_cardiomyopathy</t>
+  </si>
+  <si>
+    <t>famhist_encephalopathy</t>
+  </si>
+  <si>
+    <t>famhist_diabmell</t>
+  </si>
+  <si>
+    <t>fdsa</t>
   </si>
 </sst>
 </file>
@@ -524,7 +527,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,28 +574,28 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" t="s">
         <v>50</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>51</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>52</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>53</v>
       </c>
-      <c r="N1" t="s">
-        <v>45</v>
-      </c>
       <c r="O1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="P1" t="s">
         <v>47</v>
       </c>
       <c r="Q1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -623,29 +626,29 @@
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>49</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>49</v>
       </c>
-      <c r="M2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2">
-        <v>2</v>
-      </c>
-      <c r="O2">
-        <v>2</v>
-      </c>
-      <c r="P2">
-        <v>2</v>
-      </c>
-      <c r="Q2">
-        <v>2</v>
+      <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -677,28 +680,28 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" t="s">
         <v>49</v>
       </c>
-      <c r="K3" t="s">
-        <v>27</v>
-      </c>
       <c r="L3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" t="s">
         <v>49</v>
       </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -730,7 +733,7 @@
         <v>8</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="K4" t="s">
         <v>27</v>
@@ -741,17 +744,17 @@
       <c r="M4" t="s">
         <v>27</v>
       </c>
-      <c r="N4">
-        <v>2</v>
-      </c>
-      <c r="O4">
-        <v>2</v>
-      </c>
-      <c r="P4">
-        <v>2</v>
-      </c>
-      <c r="Q4">
-        <v>2</v>
+      <c r="N4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -782,8 +785,8 @@
       <c r="I5" t="s">
         <v>44</v>
       </c>
-      <c r="J5" t="s">
-        <v>27</v>
+      <c r="J5">
+        <v>4</v>
       </c>
       <c r="K5" t="s">
         <v>27</v>
@@ -795,16 +798,16 @@
         <v>27</v>
       </c>
       <c r="N5">
-        <v>4</v>
-      </c>
-      <c r="O5">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
+        <v>49</v>
       </c>
       <c r="P5">
         <v>4</v>
       </c>
-      <c r="Q5">
-        <v>4</v>
+      <c r="Q5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -847,17 +850,17 @@
       <c r="M6" t="s">
         <v>27</v>
       </c>
-      <c r="N6">
-        <v>5</v>
-      </c>
-      <c r="O6">
-        <v>5</v>
-      </c>
-      <c r="P6">
-        <v>5</v>
-      </c>
-      <c r="Q6">
-        <v>5</v>
+      <c r="N6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>